<commit_message>
OR update and Test data update
</commit_message>
<xml_diff>
--- a/Testdata/LiveRef/SearchPublications/SearchPublicationsPage_Data.xlsx
+++ b/Testdata/LiveRef/SearchPublications/SearchPublicationsPage_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\LiveRef\SearchPublications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265B622A-0C23-47C4-BE7B-82DC859FDFFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C06E03-AC97-4DE0-8CF9-803A9975586E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,12 +73,6 @@
     <t>scenario1</t>
   </si>
   <si>
-    <t>NR_population</t>
-  </si>
-  <si>
-    <t>NR_population_count</t>
-  </si>
-  <si>
     <t>RRMM_population</t>
   </si>
   <si>
@@ -107,6 +101,12 @@
   </si>
   <si>
     <t>RUNX1+ AML_population_count</t>
+  </si>
+  <si>
+    <t>TRMM_population</t>
+  </si>
+  <si>
+    <t>TRMM_population_count</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,13 +492,13 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -506,61 +506,61 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>